<commit_message>
Changes to format the datetime column as a pandas datetime column
</commit_message>
<xml_diff>
--- a/files/Ene022020.xlsx
+++ b/files/Ene022020.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Google Drive\WORK\ExcelsStuff\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A9EAF1-40E2-41E5-B9FE-41FDB2949684}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5DDF64-3E63-41EC-AEF3-19F6E21FB648}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2G" sheetId="2" r:id="rId1"/>
     <sheet name="3G" sheetId="3" r:id="rId2"/>
     <sheet name="4G" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_02_enero_jueves" localSheetId="0">'2G'!$A$1:$T$29804</definedName>
@@ -27,9 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -71,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9768" uniqueCount="2354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9773" uniqueCount="2359">
   <si>
     <t>RAT</t>
   </si>
@@ -7133,6 +7132,21 @@
   </si>
   <si>
     <t>ju. ene. 2 13:51:27 2020</t>
+  </si>
+  <si>
+    <t>IMSI 4G</t>
+  </si>
+  <si>
+    <t>IMEI 2G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMEI 3G </t>
+  </si>
+  <si>
+    <t>FRECUENCIA 2G</t>
+  </si>
+  <si>
+    <t>FRECUENCIA 3G</t>
   </si>
 </sst>
 </file>
@@ -7565,8 +7579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q370"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:Q369"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26048,8 +26062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q983"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:Q982"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -75031,8 +75045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:Q75"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -75158,7 +75172,7 @@
         <v>925</v>
       </c>
       <c r="E3" s="3">
-        <v>740010179029118</v>
+        <v>740010165047416</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" t="s">
@@ -78661,4 +78675,43 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CCBC3D-90B9-4B61-84D4-8764838016EC}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2354</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2357</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2355</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2358</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Conexion con archivos UI
</commit_message>
<xml_diff>
--- a/files/Ene022020.xlsx
+++ b/files/Ene022020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Google Drive\WORK\ExcelsStuff\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFFD94E-BA17-430E-A7D1-90938DFE3B33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7F4F45-5E2A-47C1-83AE-19C98019F45E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2G" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9773" uniqueCount="2359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9781" uniqueCount="2363">
   <si>
     <t>RAT</t>
   </si>
@@ -7147,6 +7147,18 @@
   </si>
   <si>
     <t>FRECUENCIA 3G</t>
+  </si>
+  <si>
+    <t>(32,1),(324,2)</t>
+  </si>
+  <si>
+    <t>FRECUENCIA IMSI</t>
+  </si>
+  <si>
+    <t>IMSIS</t>
+  </si>
+  <si>
+    <t>CANTIDAD IMSI</t>
   </si>
 </sst>
 </file>
@@ -7580,7 +7592,7 @@
   <dimension ref="A1:Q370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F10" sqref="A10:XFD10"/>
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7713,7 +7725,7 @@
         <v>740010164262704</v>
       </c>
       <c r="F3" s="3">
-        <v>357287085897934</v>
+        <v>868789022187230</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
@@ -7763,7 +7775,7 @@
         <v>740010171543395</v>
       </c>
       <c r="F4" s="3">
-        <v>868789022837768</v>
+        <v>868789022187230</v>
       </c>
       <c r="G4" t="s">
         <v>34</v>
@@ -7813,7 +7825,7 @@
         <v>740010171532713</v>
       </c>
       <c r="F5" s="3">
-        <v>864180034912118</v>
+        <v>868789022187230</v>
       </c>
       <c r="G5" t="s">
         <v>38</v>
@@ -7863,7 +7875,7 @@
         <v>740010180400321</v>
       </c>
       <c r="F6" s="3">
-        <v>354200100800091</v>
+        <v>868789022187230</v>
       </c>
       <c r="G6" t="s">
         <v>40</v>
@@ -7913,7 +7925,7 @@
         <v>740010177429093</v>
       </c>
       <c r="F7" s="3">
-        <v>358355100073747</v>
+        <v>868789022187230</v>
       </c>
       <c r="G7" t="s">
         <v>42</v>
@@ -78682,10 +78694,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CCBC3D-90B9-4B61-84D4-8764838016EC}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -78695,9 +78707,10 @@
     <col min="3" max="3" width="7.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2354</v>
       </c>
@@ -78712,6 +78725,72 @@
       </c>
       <c r="E1" t="s">
         <v>2356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2360</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2361</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>32</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2359</v>
+      </c>
+      <c r="G9" s="2">
+        <v>32324</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>